<commit_message>
Updates the Invoicing documentation
</commit_message>
<xml_diff>
--- a/Invoicing/Expected Results.xlsx
+++ b/Invoicing/Expected Results.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafaelGuzman\Personal\Documentation\Invoicing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafaelGuzman\Personal\RPA Showcase\rpa-showcase-docs\Invoicing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332E5B0F-17F8-4BC8-B58C-8697F528EF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5771CE0-9164-44FC-9BDD-BEB719B27520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoices" sheetId="1" r:id="rId1"/>
+    <sheet name="Customers" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="82">
   <si>
     <t>Client</t>
   </si>
@@ -33,18 +34,9 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Invoice date</t>
-  </si>
-  <si>
-    <t>Due date</t>
-  </si>
-  <si>
     <t>Payment Interval</t>
   </si>
   <si>
-    <t>Payment method</t>
-  </si>
-  <si>
     <t>Voucher Type</t>
   </si>
   <si>
@@ -144,9 +136,6 @@
     <t>60 days</t>
   </si>
   <si>
-    <t>International Genetic Technologies Inc.</t>
-  </si>
-  <si>
     <t>Skynet St. 12, Los Angeles, California</t>
   </si>
   <si>
@@ -255,12 +244,27 @@
     <t>Message</t>
   </si>
   <si>
+    <t>Payment Method</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>Invoice Date</t>
+  </si>
+  <si>
+    <t>International Genetic Technologies, Inc.</t>
+  </si>
+  <si>
     <t>Success</t>
   </si>
   <si>
     <t>Business Exception</t>
   </si>
   <si>
+    <t>Invalid due date</t>
+  </si>
+  <si>
     <t>Invalid invoice number.</t>
   </si>
   <si>
@@ -268,9 +272,6 @@
   </si>
   <si>
     <t>Invoice amount greater than $30,000</t>
-  </si>
-  <si>
-    <t>Invalid due date</t>
   </si>
 </sst>
 </file>
@@ -371,7 +372,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFB7B7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -385,7 +386,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
+          <bgColor rgb="FFFFB7B7"/>
         </patternFill>
       </fill>
     </dxf>
@@ -696,14 +697,14 @@
   <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P19" sqref="P19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" style="1" customWidth="1"/>
@@ -717,13 +718,13 @@
     <col min="13" max="13" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -732,43 +733,43 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -776,10 +777,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <v>45054</v>
@@ -788,25 +789,25 @@
         <v>45420</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M2" s="1">
         <v>4</v>
@@ -820,7 +821,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="L3" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M3" s="1">
         <v>9</v>
@@ -831,7 +832,7 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="L4" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M4" s="1">
         <v>10</v>
@@ -844,7 +845,7 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="L5" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M5" s="1">
         <v>2</v>
@@ -856,10 +857,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D6" s="2">
         <v>45054</v>
@@ -868,25 +869,25 @@
         <v>44903</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="I6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M6" s="1">
         <v>1</v>
@@ -896,14 +897,14 @@
         <v>77</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="L7" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="M7" s="1">
         <v>3</v>
@@ -917,10 +918,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D8" s="2">
         <v>45054</v>
@@ -929,25 +930,25 @@
         <v>45146</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="L8" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M8" s="1">
         <v>1</v>
@@ -962,10 +963,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2">
         <v>45055</v>
@@ -974,25 +975,25 @@
         <v>45269</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="L9" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M9" s="1">
         <v>9</v>
@@ -1006,7 +1007,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="L10" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M10" s="1">
         <v>2</v>
@@ -1017,7 +1018,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="L11" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="M11" s="1">
         <v>12</v>
@@ -1031,10 +1032,10 @@
         <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D12" s="2">
         <v>45055</v>
@@ -1043,25 +1044,25 @@
         <v>45178</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="L12" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M12" s="1">
         <v>2</v>
@@ -1075,7 +1076,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="L13" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M13" s="1">
         <v>3</v>
@@ -1086,7 +1087,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="L14" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M14" s="1">
         <v>9</v>
@@ -1097,7 +1098,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="L15" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M15" s="1">
         <v>8</v>
@@ -1110,7 +1111,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="L16" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M16" s="1">
         <v>4</v>
@@ -1122,10 +1123,10 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D17" s="2">
         <v>45055</v>
@@ -1134,25 +1135,25 @@
         <v>45269</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="I17" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M17" s="1">
         <v>7</v>
@@ -1168,7 +1169,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="L18" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="M18" s="1">
         <v>1</v>
@@ -1180,10 +1181,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D19" s="2">
         <v>45055</v>
@@ -1192,25 +1193,25 @@
         <v>45421</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="I19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="L19" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M19" s="1">
         <v>9</v>
@@ -1224,7 +1225,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="L20" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M20" s="1">
         <v>15</v>
@@ -1237,7 +1238,7 @@
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="L21" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M21" s="1">
         <v>5</v>
@@ -1248,7 +1249,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="L22" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M22" s="1">
         <v>3</v>
@@ -1260,10 +1261,10 @@
         <v>8</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D23" s="2">
         <v>45056</v>
@@ -1272,25 +1273,25 @@
         <v>45087</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M23" s="1">
         <v>1</v>
@@ -1304,7 +1305,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="L24" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M24" s="1">
         <v>8</v>
@@ -1317,7 +1318,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="L25" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="M25" s="1">
         <v>3</v>
@@ -1329,10 +1330,10 @@
         <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D26" s="2">
         <v>45056</v>
@@ -1341,25 +1342,25 @@
         <v>45117</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="I26" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M26" s="1">
         <v>7</v>
@@ -1373,7 +1374,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="L27" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M27" s="1">
         <v>16</v>
@@ -1387,10 +1388,10 @@
         <v>10</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D28" s="2">
         <v>45056</v>
@@ -1399,25 +1400,25 @@
         <v>45514</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="I28" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M28" s="1">
         <v>9</v>
@@ -1427,14 +1428,14 @@
         <v>77</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="L29" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M29" s="1">
         <v>8</v>
@@ -1445,7 +1446,7 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="L30" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="M30" s="1">
         <v>7</v>
@@ -1457,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="2">
@@ -1467,25 +1468,25 @@
         <v>45088</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="J31" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M31" s="1">
         <v>6</v>
@@ -1495,7 +1496,7 @@
         <v>77</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1503,10 +1504,10 @@
         <v>12</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D32" s="2">
         <v>45057</v>
@@ -1515,25 +1516,25 @@
         <v>45149</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J32" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="L32" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="M32" s="1">
         <v>3</v>
@@ -1547,7 +1548,7 @@
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="L33" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M33" s="1">
         <v>11</v>
@@ -1561,10 +1562,10 @@
         <v>13</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D34" s="2">
         <v>45058</v>
@@ -1573,25 +1574,25 @@
         <v>45272</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H34" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="I34" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M34" s="1">
         <v>20</v>
@@ -1601,14 +1602,14 @@
         <v>77</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="L35" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M35" s="1">
         <v>30</v>
@@ -1619,7 +1620,7 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="L36" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M36" s="1">
         <v>25</v>
@@ -1630,7 +1631,7 @@
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="L37" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="M37" s="1">
         <v>75</v>
@@ -1644,10 +1645,10 @@
         <v>14</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D38" s="2">
         <v>45058</v>
@@ -1656,23 +1657,23 @@
         <v>45424</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="J38" s="4"/>
       <c r="K38" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M38" s="1">
         <v>13</v>
@@ -1684,14 +1685,14 @@
         <v>77</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
       <c r="L39" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="M39" s="1">
         <v>2</v>
@@ -1702,7 +1703,7 @@
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="L40" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M40" s="1">
         <v>1</v>
@@ -1714,10 +1715,10 @@
         <v>15</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D41" s="2">
         <v>45058</v>
@@ -1726,25 +1727,25 @@
         <v>45089</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="M41" s="1">
         <v>8</v>
@@ -1760,7 +1761,7 @@
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="L42" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M42" s="1">
         <v>10</v>
@@ -1773,7 +1774,7 @@
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="L43" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="M43" s="1">
         <v>5</v>
@@ -1784,7 +1785,7 @@
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="L44" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M44" s="1">
         <v>2</v>
@@ -1796,10 +1797,10 @@
         <v>16</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D45" s="2">
         <v>45058</v>
@@ -1808,25 +1809,25 @@
         <v>45057</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="M45" s="1">
         <v>2</v>
@@ -1844,22 +1845,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O1048576">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Success">
-      <formula>NOT(ISERROR(SEARCH("Success",O2)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Failure">
+      <formula>NOT(ISERROR(SEARCH("Failure",O2)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Exception">
       <formula>NOT(ISERROR(SEARCH("Exception",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Failure">
-      <formula>NOT(ISERROR(SEARCH("Failure",O2)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Success">
+      <formula>NOT(ISERROR(SEARCH("Success",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="9">
+  <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{28708D3D-AE26-4E85-B83E-3684AC78F45E}">
       <formula1>"12 days,15 days,30 days,60 days"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{C0719A99-61B1-4541-8598-3D87DBAB8CED}">
-      <formula1>"Cyberdyne Systems,Vandelay Industries,International Genetic Technologies Inc.,Umbrella Corporation,Globex,Wayne Enterprises,Stark Industries,Initech"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{49CD8C6F-3453-4F46-B4E8-FC859209FE54}">
       <formula1>"Credit,Cash,Check,Debit"</formula1>
@@ -1886,5 +1884,75 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AC75C327-C05E-4B21-A69C-236334FA94C2}">
+          <x14:formula1>
+            <xm:f>Customers!$A$1:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3:B1048576 B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73BB03D7-9363-4D58-89C4-706257FFA7A2}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update in the expected results for the invoicing case
</commit_message>
<xml_diff>
--- a/Invoicing/Expected Results.xlsx
+++ b/Invoicing/Expected Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RafaelGuzman\Personal\RPA Showcase\rpa-showcase-docs\Invoicing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5771CE0-9164-44FC-9BDD-BEB719B27520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AC1111-CBE4-4A44-9454-A3B41041E9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoices" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="83">
   <si>
     <t>Client</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>Invoice amount greater than $30,000</t>
+  </si>
+  <si>
+    <t>Invalid invoice number</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -696,9 +720,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1069,7 +1093,10 @@
       </c>
       <c r="N12" s="4"/>
       <c r="O12" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
@@ -1834,24 +1861,27 @@
       </c>
       <c r="N45" s="4"/>
       <c r="O45" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="P45" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:P45">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>NOT(ISBLANK(A2:L10000))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Failure">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failure">
       <formula>NOT(ISERROR(SEARCH("Failure",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Exception">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Exception">
       <formula>NOT(ISERROR(SEARCH("Exception",O2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Success">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Success">
       <formula>NOT(ISERROR(SEARCH("Success",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1891,7 +1921,7 @@
           <x14:formula1>
             <xm:f>Customers!$A$1:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B3:B1048576 B2</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>